<commit_message>
Stack increased; speed & distance in kmh
</commit_message>
<xml_diff>
--- a/biltema-count.xlsx
+++ b/biltema-count.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boe\Documents\BoE\git\ewarm\lpc2138-sk\arm\9.10.2\NXP\LPC213x\IAR-P213x\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A413AAFE-1B27-4A38-B1DE-C0D5850860C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE71219F-9BD7-4308-BFD7-5388953476E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6B61B452-E600-4EBA-B8C4-BD7C91B691E2}"/>
+    <workbookView xWindow="900" yWindow="885" windowWidth="21600" windowHeight="11385" xr2:uid="{6B61B452-E600-4EBA-B8C4-BD7C91B691E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Distance" sheetId="10" r:id="rId1"/>
+    <sheet name="Speed" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
   <si>
     <t>lpc2138-biltema-teraterm</t>
   </si>
@@ -235,25 +237,85 @@
     <t>y = kx +m</t>
   </si>
   <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>It_n</t>
-  </si>
-  <si>
-    <t>y = -71242x + 1,6652</t>
-  </si>
-  <si>
-    <t>vt =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -71242 * it</t>
-  </si>
-  <si>
-    <t>Ri=71242 ohm</t>
-  </si>
-  <si>
-    <t>70K</t>
+    <t>28 bits needed</t>
+  </si>
+  <si>
+    <t>km / h</t>
+  </si>
+  <si>
+    <t>distance per pulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ticks per pulse </t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>speed = 0.6 * / (N / f)</t>
+  </si>
+  <si>
+    <t>speed = 0.6 * f / N</t>
+  </si>
+  <si>
+    <t>km/h / m/s</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>dpp</t>
+  </si>
+  <si>
+    <t>kmh_ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>f * dpp</t>
+  </si>
+  <si>
+    <t>f * dpp * kmh_ms</t>
+  </si>
+  <si>
+    <t>f * dpp / t_p_p</t>
+  </si>
+  <si>
+    <t>f * dpp * kmh_ms / t_p_p</t>
+  </si>
+  <si>
+    <t>f * dpp * kmh_ms * 100</t>
+  </si>
+  <si>
+    <t>f * dpp * kmh_ms * 100/ t_p_p</t>
+  </si>
+  <si>
+    <t>0.01 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># bits </t>
+  </si>
+  <si>
+    <t>number of pulses</t>
+  </si>
+  <si>
+    <t>N * dpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ticks </t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>N/1000 * dpp</t>
   </si>
 </sst>
 </file>
@@ -278,15 +340,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -294,11 +368,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,6 +470,53 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,817 +919,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-SE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet7!$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Vt</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.3279897200349956"/>
-                  <c:y val="-0.12579906678331876"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet7!$E$5:$E$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="2">
-                  <c:v>1.0106382978723405</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.005531914893617</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0021276595744681</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99734042553191482</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98350981870635679</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.93936170212765957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.79290780141843975</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.79929078014184396</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.6562039182641668</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.48120567375886519</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.37553191489361698</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.30765957446808512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet7!$F$5:$F$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="2">
-                  <c:v>0.90927358585351159</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.88601426705515929</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.8627549482568071</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.81633678287953382</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.70330553601929069</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.56113734552396266</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.44308248769215308</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.43856123781774342</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.3787802672561037</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.32301818547171707</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.29538832512810215</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.27830804782477647</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F976-4558-94D5-40A4FE088A9D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="398305696"/>
-        <c:axId val="398297376"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="398305696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398297376"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="398297376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="398305696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-SE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-SE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.15734886264216974"/>
-                  <c:y val="7.2465733449985414E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-SE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet7!$B$42:$B$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.892E-6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.5299999999999997E-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5233333333333329E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.1683168316831681E-6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.5133333333333331E-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.4533333333333337E-6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet7!$C$42:$C$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.446</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4119999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.357</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.246</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.127</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1180000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E035-419D-ACBE-BC05DB6B6657}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="674264688"/>
-        <c:axId val="674258448"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="674264688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="674258448"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="674258448"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-SE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="674264688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-SE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2108,86 +1498,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2705,1038 +2015,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4281,83 +2559,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>42861</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5708023-681A-453E-A7C7-3194115E33A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368F8B38-F2A4-4E49-839B-9F858AD20E69}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4990,16 +3191,577 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F0FC3F-DE5A-4D78-909C-A5291776C0C5}">
-  <dimension ref="A1:S50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623EDA6-AF1B-4B7D-B9EF-0A62D37B7699}">
+  <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="8"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="16">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H8" s="16">
+        <f>$D$5*$D$4*$D$6*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9">
+        <f>ROUNDUP(LOG(D8,2),0)</f>
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <f>ROUNDUP(LOG(F8,2),0)</f>
+        <v>-11</v>
+      </c>
+      <c r="H9" t="e">
+        <f>ROUNDUP(LOG(H8,2),0)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="27"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
+        <v>1</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22">
+        <f>$D$8*$B13</f>
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22">
+        <f>$F$8*$B13</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="31">
+        <f>$H$8/$B13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
+        <v>100</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22">
+        <f t="shared" ref="D14:D17" si="0">$D$8*$B14</f>
+        <v>60</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22">
+        <f t="shared" ref="F14:F17" si="1">$F$8*$B14</f>
+        <v>0.06</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="31">
+        <f t="shared" ref="H14:H17" si="2">$H$8/$B14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="30">
+        <v>10000</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="32">
+        <v>65535</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="22">
+        <f t="shared" si="0"/>
+        <v>39321</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="22">
+        <f t="shared" si="1"/>
+        <v>39.320999999999998</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DBD9275-8E28-4C5A-AF74-EB5752901F53}">
+  <dimension ref="A2:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="8"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="12">
+        <v>14740000</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <f>D2/D3</f>
+        <v>1052857.142857143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="16">
+        <f>$D$4*$D$5</f>
+        <v>631714.2857142858</v>
+      </c>
+      <c r="F8" s="16">
+        <f>$D$5*$D$4*$D$6</f>
+        <v>2274171.4285714291</v>
+      </c>
+      <c r="H8" s="16">
+        <f>$D$5*$D$4*$D$6*100</f>
+        <v>227417142.85714293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9">
+        <f>ROUNDUP(LOG(D8,2),0)</f>
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <f>ROUNDUP(LOG(F8,2),0)</f>
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <f>ROUNDUP(LOG(H8,2),0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="27"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22">
+        <f>$D$8/$B13</f>
+        <v>0.63171428571428578</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22">
+        <f>$F$8/$B13</f>
+        <v>2.274171428571429</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="31">
+        <f>$H$8/$B13</f>
+        <v>227.41714285714292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="30">
+        <v>500000</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22">
+        <f t="shared" ref="D14:D17" si="0">$D$8/$B14</f>
+        <v>1.2634285714285716</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22">
+        <f t="shared" ref="F14:H17" si="1">$F$8/$B14</f>
+        <v>4.5483428571428579</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="31">
+        <f t="shared" ref="H14:H17" si="2">$H$8/$B14</f>
+        <v>454.83428571428584</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
+        <v>100000</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22">
+        <f t="shared" si="0"/>
+        <v>6.3171428571428576</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22">
+        <f t="shared" si="1"/>
+        <v>22.741714285714291</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="31">
+        <f t="shared" si="2"/>
+        <v>2274.1714285714293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="30">
+        <v>50000</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22">
+        <f t="shared" si="0"/>
+        <v>12.634285714285715</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22">
+        <f t="shared" si="1"/>
+        <v>45.483428571428583</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="31">
+        <f t="shared" si="2"/>
+        <v>4548.3428571428585</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="32">
+        <v>10000</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34">
+        <f t="shared" si="0"/>
+        <v>63.171428571428578</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34">
+        <f t="shared" si="1"/>
+        <v>227.41714285714292</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35">
+        <f t="shared" si="2"/>
+        <v>22741.714285714294</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F0FC3F-DE5A-4D78-909C-A5291776C0C5}">
+  <dimension ref="A1:S52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -5018,12 +3780,12 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
         <v>33</v>
@@ -6171,6 +4933,21 @@
       <c r="A50">
         <f>INT(A49)</f>
         <v>227417142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f>LOG(A50,2)</f>
+        <v>27.760765763312818</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>DEC2HEX(A50,8)</f>
+        <v>0D8E1C36</v>
       </c>
     </row>
   </sheetData>
@@ -6182,7 +4959,187 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43748CBE-D409-494C-B676-FD84B2786DF8}">
+  <dimension ref="B2:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="12">
+        <v>14740000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <f>D2/D3</f>
+        <v>1052857.142857143</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>1000000</v>
+      </c>
+      <c r="F8">
+        <v>500000</v>
+      </c>
+      <c r="G8">
+        <v>100000</v>
+      </c>
+      <c r="H8">
+        <v>50000</v>
+      </c>
+      <c r="I8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <f>$D$6*$D$4/E$8</f>
+        <v>0.63171428571428578</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:I11" si="0">$D$6*$D$4/F$8</f>
+        <v>1.2634285714285716</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>6.3171428571428576</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>12.634285714285715</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>63.171428571428578</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <f>$D$14*$D$6*$D$4/E$8</f>
+        <v>2.274171428571429</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:I12" si="1">$D$14*$D$6*$D$4/F$8</f>
+        <v>4.5483428571428579</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>22.741714285714291</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>45.483428571428583</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>227.41714285714292</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <f>D9*D14</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787509D4-8F11-4FA5-92CA-65E55090F2E3}">
   <dimension ref="B3:H20"/>
   <sheetViews>
@@ -6359,11 +5316,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B96623D-FF22-441A-ADB1-778F8D735941}">
   <dimension ref="B4:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G36"/>
     </sheetView>
   </sheetViews>
@@ -6771,407 +5728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D73B2AD-BB0B-486E-B80B-0CC1B015622A}">
-  <dimension ref="A4:G57"/>
-  <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="C5">
-        <v>9.4000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="C6">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>9.5000000000000005E-6</v>
-      </c>
-      <c r="C7">
-        <v>0.19</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E6:E18" si="0">B7/B$5</f>
-        <v>1.0106382978723405</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F6:F18" si="1">(2-C7)/(2-C$5)</f>
-        <v>0.90927358585351159</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>9.4520000000000003E-6</v>
-      </c>
-      <c r="C8">
-        <v>0.23630000000000001</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1.005531914893617</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.88601426705515929</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>9.4200000000000013E-6</v>
-      </c>
-      <c r="C9">
-        <v>0.28260000000000002</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.0021276595744681</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0.8627549482568071</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>9.3749999999999992E-6</v>
-      </c>
-      <c r="C10">
-        <v>0.375</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0.99734042553191482</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.81633678287953382</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>9.2449922958397537E-6</v>
-      </c>
-      <c r="C11">
-        <v>0.6</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0.98350981870635679</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.70330553601929069</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>8.8300000000000002E-6</v>
-      </c>
-      <c r="C12">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0.93936170212765957</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.56113734552396266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>7.4533333333333337E-6</v>
-      </c>
-      <c r="C13">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0.79290780141843975</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.44308248769215308</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>7.5133333333333331E-6</v>
-      </c>
-      <c r="C14">
-        <v>1.127</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0.79929078014184396</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.43856123781774342</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>6.1683168316831681E-6</v>
-      </c>
-      <c r="C15">
-        <v>1.246</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0.6562039182641668</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0.3787802672561037</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>4.5233333333333329E-6</v>
-      </c>
-      <c r="C16">
-        <v>1.357</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0.48120567375886519</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.32301818547171707</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>3.5299999999999997E-6</v>
-      </c>
-      <c r="C17">
-        <v>1.4119999999999999</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0.37553191489361698</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>0.29538832512810215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>2.892E-6</v>
-      </c>
-      <c r="C18">
-        <v>1.446</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0.30765957446808512</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>0.27830804782477647</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>1.756</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27">
-        <v>1.6652</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>2.892E-6</v>
-      </c>
-      <c r="C42">
-        <v>1.446</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>3.5299999999999997E-6</v>
-      </c>
-      <c r="C43">
-        <v>1.4119999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>4.5233333333333329E-6</v>
-      </c>
-      <c r="C44">
-        <v>1.357</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>6.1683168316831681E-6</v>
-      </c>
-      <c r="C45">
-        <v>1.246</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>7.5133333333333331E-6</v>
-      </c>
-      <c r="C46">
-        <v>1.127</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>7.4533333333333337E-6</v>
-      </c>
-      <c r="C47">
-        <v>1.1180000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>8.8300000000000002E-6</v>
-      </c>
-      <c r="C48">
-        <v>0.88300000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>9.2449922958397537E-6</v>
-      </c>
-      <c r="C49">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>9.3749999999999992E-6</v>
-      </c>
-      <c r="C50">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>9.4200000000000013E-6</v>
-      </c>
-      <c r="C51">
-        <v>0.28260000000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>9.4520000000000003E-6</v>
-      </c>
-      <c r="C52">
-        <v>0.23630000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>9.5000000000000005E-6</v>
-      </c>
-      <c r="C53">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="C54">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="C55">
-        <v>9.4000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B42:C55">
-    <sortCondition descending="1" ref="C42:C55"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF3B26C-6B3B-4B7D-AA15-714311842B53}">
   <dimension ref="A3:C9"/>
   <sheetViews>

</xml_diff>